<commit_message>
[#1] excel message bundle 로 연동
</commit_message>
<xml_diff>
--- a/jcommune-service/src/main/resources/messageBundle.xlsx
+++ b/jcommune-service/src/main/resources/messageBundle.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="600" windowWidth="27735" windowHeight="11475"/>
+    <workbookView xWindow="3260" yWindow="1000" windowWidth="27740" windowHeight="11480"/>
   </bookViews>
   <sheets>
     <sheet name="message" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2305" uniqueCount="1623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2305" uniqueCount="1625">
   <si>
     <t>label.contact.type</t>
   </si>
@@ -4888,26 +4893,55 @@
   <si>
     <t>ru</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ko</t>
+  </si>
+  <si>
+    <t>한국어</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="굴림"/>
+      <family val="2"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4927,18 +4961,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5239,18 +5284,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E461"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="D165" sqref="D165"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="31.625" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
     <col min="2" max="2" width="35.5" customWidth="1"/>
-    <col min="3" max="3" width="28.125" customWidth="1"/>
-    <col min="4" max="4" width="37.875" customWidth="1"/>
-    <col min="5" max="5" width="40.125" customWidth="1"/>
+    <col min="3" max="3" width="28.1640625" customWidth="1"/>
+    <col min="4" max="4" width="37.83203125" customWidth="1"/>
+    <col min="5" max="5" width="40.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>1618</v>
       </c>
@@ -5267,7 +5314,7 @@
         <v>1622</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5284,7 +5331,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -5301,7 +5348,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -5318,7 +5365,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -5335,7 +5382,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -5352,7 +5399,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -5369,7 +5416,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -5386,7 +5433,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -5403,7 +5450,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -5420,7 +5467,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -5437,7 +5484,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -5454,7 +5501,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -5471,7 +5518,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -5488,7 +5535,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -5505,7 +5552,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -5522,7 +5569,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -5539,7 +5586,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -5556,7 +5603,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -5573,7 +5620,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>68</v>
       </c>
@@ -5590,7 +5637,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>71</v>
       </c>
@@ -5607,7 +5654,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -5624,7 +5671,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>79</v>
       </c>
@@ -5641,7 +5688,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>83</v>
       </c>
@@ -5658,7 +5705,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>87</v>
       </c>
@@ -5675,7 +5722,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>90</v>
       </c>
@@ -5692,7 +5739,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>94</v>
       </c>
@@ -5709,7 +5756,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>98</v>
       </c>
@@ -5726,7 +5773,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>102</v>
       </c>
@@ -5743,7 +5790,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>106</v>
       </c>
@@ -5760,7 +5807,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>110</v>
       </c>
@@ -5777,7 +5824,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>114</v>
       </c>
@@ -5794,7 +5841,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>118</v>
       </c>
@@ -5811,7 +5858,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>119</v>
       </c>
@@ -5828,7 +5875,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>121</v>
       </c>
@@ -5845,7 +5892,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>124</v>
       </c>
@@ -5862,7 +5909,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>128</v>
       </c>
@@ -5879,7 +5926,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>132</v>
       </c>
@@ -5896,7 +5943,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>136</v>
       </c>
@@ -5913,7 +5960,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>140</v>
       </c>
@@ -5930,7 +5977,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>144</v>
       </c>
@@ -5947,7 +5994,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>147</v>
       </c>
@@ -5964,7 +6011,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>151</v>
       </c>
@@ -5981,7 +6028,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>155</v>
       </c>
@@ -5998,7 +6045,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>159</v>
       </c>
@@ -6015,7 +6062,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>163</v>
       </c>
@@ -6032,7 +6079,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>167</v>
       </c>
@@ -6049,7 +6096,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>170</v>
       </c>
@@ -6066,7 +6113,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>174</v>
       </c>
@@ -6083,7 +6130,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>178</v>
       </c>
@@ -6100,7 +6147,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>182</v>
       </c>
@@ -6117,7 +6164,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>186</v>
       </c>
@@ -6134,7 +6181,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>190</v>
       </c>
@@ -6151,7 +6198,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>193</v>
       </c>
@@ -6168,7 +6215,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>196</v>
       </c>
@@ -6185,7 +6232,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>200</v>
       </c>
@@ -6202,7 +6249,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>204</v>
       </c>
@@ -6219,7 +6266,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>208</v>
       </c>
@@ -6236,7 +6283,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>212</v>
       </c>
@@ -6253,7 +6300,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>216</v>
       </c>
@@ -6270,7 +6317,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>220</v>
       </c>
@@ -6287,7 +6334,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>223</v>
       </c>
@@ -6304,7 +6351,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>227</v>
       </c>
@@ -6321,7 +6368,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
         <v>231</v>
       </c>
@@ -6338,7 +6385,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
         <v>235</v>
       </c>
@@ -6355,7 +6402,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
         <v>237</v>
       </c>
@@ -6372,7 +6419,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>241</v>
       </c>
@@ -6389,7 +6436,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>245</v>
       </c>
@@ -6406,7 +6453,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
         <v>249</v>
       </c>
@@ -6423,7 +6470,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>252</v>
       </c>
@@ -6440,7 +6487,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>256</v>
       </c>
@@ -6457,7 +6504,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>260</v>
       </c>
@@ -6474,7 +6521,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
         <v>264</v>
       </c>
@@ -6491,7 +6538,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>268</v>
       </c>
@@ -6508,7 +6555,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>272</v>
       </c>
@@ -6525,7 +6572,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>276</v>
       </c>
@@ -6542,7 +6589,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
         <v>280</v>
       </c>
@@ -6559,7 +6606,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
         <v>284</v>
       </c>
@@ -6576,7 +6623,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
         <v>288</v>
       </c>
@@ -6593,7 +6640,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
         <v>292</v>
       </c>
@@ -6610,7 +6657,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
         <v>296</v>
       </c>
@@ -6627,7 +6674,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>300</v>
       </c>
@@ -6644,7 +6691,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>301</v>
       </c>
@@ -6661,7 +6708,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5">
       <c r="A84" t="s">
         <v>304</v>
       </c>
@@ -6678,7 +6725,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5">
       <c r="A85" t="s">
         <v>308</v>
       </c>
@@ -6695,7 +6742,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
         <v>311</v>
       </c>
@@ -6712,7 +6759,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
         <v>315</v>
       </c>
@@ -6729,7 +6776,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
         <v>319</v>
       </c>
@@ -6746,7 +6793,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
         <v>323</v>
       </c>
@@ -6763,7 +6810,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>327</v>
       </c>
@@ -6780,7 +6827,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>331</v>
       </c>
@@ -6797,7 +6844,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>335</v>
       </c>
@@ -6814,7 +6861,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
         <v>339</v>
       </c>
@@ -6831,7 +6878,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>343</v>
       </c>
@@ -6848,7 +6895,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
         <v>347</v>
       </c>
@@ -6865,7 +6912,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
         <v>348</v>
       </c>
@@ -6882,7 +6929,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5">
       <c r="A97" t="s">
         <v>352</v>
       </c>
@@ -6899,7 +6946,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
         <v>356</v>
       </c>
@@ -6916,7 +6963,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5">
       <c r="A99" t="s">
         <v>360</v>
       </c>
@@ -6933,7 +6980,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5">
       <c r="A100" t="s">
         <v>364</v>
       </c>
@@ -6950,7 +6997,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5">
       <c r="A101" t="s">
         <v>368</v>
       </c>
@@ -6967,7 +7014,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5">
       <c r="A102" t="s">
         <v>372</v>
       </c>
@@ -6984,7 +7031,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5">
       <c r="A103" t="s">
         <v>376</v>
       </c>
@@ -7001,7 +7048,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5">
       <c r="A104" t="s">
         <v>379</v>
       </c>
@@ -7018,7 +7065,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5">
       <c r="A105" t="s">
         <v>383</v>
       </c>
@@ -7035,7 +7082,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5">
       <c r="A106" t="s">
         <v>385</v>
       </c>
@@ -7052,7 +7099,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5">
       <c r="A107" t="s">
         <v>389</v>
       </c>
@@ -7069,7 +7116,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5">
       <c r="A108" t="s">
         <v>393</v>
       </c>
@@ -7086,7 +7133,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5">
       <c r="A109" t="s">
         <v>397</v>
       </c>
@@ -7103,7 +7150,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5">
       <c r="A110" t="s">
         <v>400</v>
       </c>
@@ -7120,7 +7167,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5">
       <c r="A111" t="s">
         <v>404</v>
       </c>
@@ -7137,7 +7184,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5">
       <c r="A112" t="s">
         <v>408</v>
       </c>
@@ -7154,7 +7201,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5">
       <c r="A113" t="s">
         <v>412</v>
       </c>
@@ -7171,7 +7218,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5">
       <c r="A114" t="s">
         <v>416</v>
       </c>
@@ -7188,7 +7235,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5">
       <c r="A115" t="s">
         <v>420</v>
       </c>
@@ -7205,7 +7252,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5">
       <c r="A116" t="s">
         <v>421</v>
       </c>
@@ -7222,7 +7269,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5">
       <c r="A117" t="s">
         <v>425</v>
       </c>
@@ -7239,7 +7286,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5">
       <c r="A118" t="s">
         <v>429</v>
       </c>
@@ -7256,7 +7303,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5">
       <c r="A119" t="s">
         <v>433</v>
       </c>
@@ -7273,7 +7320,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5">
       <c r="A120" t="s">
         <v>437</v>
       </c>
@@ -7290,7 +7337,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5">
       <c r="A121" t="s">
         <v>441</v>
       </c>
@@ -7307,7 +7354,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5">
       <c r="A122" t="s">
         <v>445</v>
       </c>
@@ -7324,7 +7371,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5">
       <c r="A123" t="s">
         <v>449</v>
       </c>
@@ -7341,7 +7388,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5">
       <c r="A124" t="s">
         <v>452</v>
       </c>
@@ -7358,7 +7405,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5">
       <c r="A125" t="s">
         <v>456</v>
       </c>
@@ -7375,7 +7422,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5">
       <c r="A126" t="s">
         <v>457</v>
       </c>
@@ -7392,7 +7439,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5">
       <c r="A127" t="s">
         <v>461</v>
       </c>
@@ -7409,7 +7456,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5">
       <c r="A128" t="s">
         <v>465</v>
       </c>
@@ -7426,7 +7473,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5">
       <c r="A129" t="s">
         <v>469</v>
       </c>
@@ -7443,7 +7490,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5">
       <c r="A130" t="s">
         <v>473</v>
       </c>
@@ -7460,7 +7507,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5">
       <c r="A131" t="s">
         <v>477</v>
       </c>
@@ -7477,7 +7524,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5">
       <c r="A132" t="s">
         <v>481</v>
       </c>
@@ -7494,7 +7541,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5">
       <c r="A133" t="s">
         <v>485</v>
       </c>
@@ -7511,7 +7558,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5">
       <c r="A134" t="s">
         <v>489</v>
       </c>
@@ -7528,7 +7575,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5">
       <c r="A135" t="s">
         <v>493</v>
       </c>
@@ -7545,7 +7592,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5">
       <c r="A136" t="s">
         <v>497</v>
       </c>
@@ -7562,7 +7609,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5">
       <c r="A137" t="s">
         <v>501</v>
       </c>
@@ -7579,7 +7626,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5">
       <c r="A138" t="s">
         <v>505</v>
       </c>
@@ -7596,7 +7643,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5">
       <c r="A139" t="s">
         <v>507</v>
       </c>
@@ -7613,7 +7660,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5">
       <c r="A140" t="s">
         <v>511</v>
       </c>
@@ -7630,7 +7677,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5">
       <c r="A141" t="s">
         <v>514</v>
       </c>
@@ -7647,7 +7694,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5">
       <c r="A142" t="s">
         <v>518</v>
       </c>
@@ -7664,7 +7711,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5">
       <c r="A143" t="s">
         <v>522</v>
       </c>
@@ -7681,7 +7728,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5">
       <c r="A144" t="s">
         <v>526</v>
       </c>
@@ -7698,7 +7745,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5">
       <c r="A145" t="s">
         <v>530</v>
       </c>
@@ -7715,7 +7762,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5">
       <c r="A146" t="s">
         <v>533</v>
       </c>
@@ -7732,7 +7779,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5">
       <c r="A147" t="s">
         <v>537</v>
       </c>
@@ -7749,7 +7796,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5">
       <c r="A148" t="s">
         <v>541</v>
       </c>
@@ -7766,7 +7813,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5">
       <c r="A149" t="s">
         <v>545</v>
       </c>
@@ -7783,7 +7830,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5">
       <c r="A150" t="s">
         <v>548</v>
       </c>
@@ -7800,7 +7847,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5">
       <c r="A151" t="s">
         <v>552</v>
       </c>
@@ -7817,7 +7864,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5">
       <c r="A152" t="s">
         <v>556</v>
       </c>
@@ -7834,7 +7881,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5">
       <c r="A153" t="s">
         <v>560</v>
       </c>
@@ -7851,7 +7898,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5">
       <c r="A154" t="s">
         <v>564</v>
       </c>
@@ -7868,7 +7915,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5">
       <c r="A155" t="s">
         <v>568</v>
       </c>
@@ -7885,7 +7932,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5">
       <c r="A156" t="s">
         <v>571</v>
       </c>
@@ -7902,7 +7949,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5">
       <c r="A157" t="s">
         <v>573</v>
       </c>
@@ -7919,7 +7966,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5">
       <c r="A158" t="s">
         <v>577</v>
       </c>
@@ -7936,7 +7983,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5">
       <c r="A159" t="s">
         <v>581</v>
       </c>
@@ -7953,7 +8000,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5">
       <c r="A160" t="s">
         <v>585</v>
       </c>
@@ -7970,7 +8017,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5">
       <c r="A161" t="s">
         <v>589</v>
       </c>
@@ -7987,7 +8034,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5">
       <c r="A162" t="s">
         <v>593</v>
       </c>
@@ -8004,7 +8051,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5">
       <c r="A163" t="s">
         <v>597</v>
       </c>
@@ -8021,7 +8068,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5">
       <c r="A164" t="s">
         <v>601</v>
       </c>
@@ -8031,14 +8078,14 @@
       <c r="C164" t="s">
         <v>270</v>
       </c>
-      <c r="D164" t="s">
-        <v>602</v>
+      <c r="D164" s="1" t="s">
+        <v>1365</v>
       </c>
       <c r="E164" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5">
       <c r="A165" t="s">
         <v>604</v>
       </c>
@@ -8055,7 +8102,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5">
       <c r="A166" t="s">
         <v>605</v>
       </c>
@@ -8072,7 +8119,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5">
       <c r="A167" t="s">
         <v>606</v>
       </c>
@@ -8089,7 +8136,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5">
       <c r="A168" t="s">
         <v>610</v>
       </c>
@@ -8106,7 +8153,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5">
       <c r="A169" t="s">
         <v>614</v>
       </c>
@@ -8123,7 +8170,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5">
       <c r="A170" t="s">
         <v>617</v>
       </c>
@@ -8140,7 +8187,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5">
       <c r="A171" t="s">
         <v>621</v>
       </c>
@@ -8157,7 +8204,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5">
       <c r="A172" t="s">
         <v>626</v>
       </c>
@@ -8174,7 +8221,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5">
       <c r="A173" t="s">
         <v>630</v>
       </c>
@@ -8191,7 +8238,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5">
       <c r="A174" t="s">
         <v>633</v>
       </c>
@@ -8208,7 +8255,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5">
       <c r="A175" t="s">
         <v>637</v>
       </c>
@@ -8225,7 +8272,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5">
       <c r="A176" t="s">
         <v>641</v>
       </c>
@@ -8242,7 +8289,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5">
       <c r="A177" t="s">
         <v>645</v>
       </c>
@@ -8259,7 +8306,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5">
       <c r="A178" t="s">
         <v>649</v>
       </c>
@@ -8276,7 +8323,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5">
       <c r="A179" t="s">
         <v>653</v>
       </c>
@@ -8286,14 +8333,14 @@
       <c r="C179" t="s">
         <v>654</v>
       </c>
-      <c r="D179" t="s">
-        <v>602</v>
+      <c r="D179" s="1" t="s">
+        <v>1624</v>
       </c>
       <c r="E179" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5">
       <c r="A180" t="s">
         <v>656</v>
       </c>
@@ -8310,7 +8357,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5">
       <c r="A181" t="s">
         <v>657</v>
       </c>
@@ -8327,7 +8374,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5">
       <c r="A182" t="s">
         <v>658</v>
       </c>
@@ -8344,7 +8391,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5">
       <c r="A183" t="s">
         <v>662</v>
       </c>
@@ -8361,7 +8408,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5">
       <c r="A184" t="s">
         <v>665</v>
       </c>
@@ -8378,7 +8425,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5">
       <c r="A185" t="s">
         <v>669</v>
       </c>
@@ -8395,7 +8442,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5">
       <c r="A186" t="s">
         <v>673</v>
       </c>
@@ -8412,7 +8459,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5">
       <c r="A187" t="s">
         <v>677</v>
       </c>
@@ -8429,7 +8476,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:5">
       <c r="A188" t="s">
         <v>681</v>
       </c>
@@ -8446,7 +8493,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:5">
       <c r="A189" t="s">
         <v>685</v>
       </c>
@@ -8463,7 +8510,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:5">
       <c r="A190" t="s">
         <v>688</v>
       </c>
@@ -8480,7 +8527,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:5">
       <c r="A191" t="s">
         <v>689</v>
       </c>
@@ -8497,7 +8544,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5">
       <c r="A192" t="s">
         <v>693</v>
       </c>
@@ -8514,7 +8561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5">
       <c r="A193" t="s">
         <v>695</v>
       </c>
@@ -8531,7 +8578,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5">
       <c r="A194" t="s">
         <v>696</v>
       </c>
@@ -8548,7 +8595,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5">
       <c r="A195" t="s">
         <v>700</v>
       </c>
@@ -8565,7 +8612,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5">
       <c r="A196" t="s">
         <v>703</v>
       </c>
@@ -8582,7 +8629,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5">
       <c r="A197" t="s">
         <v>707</v>
       </c>
@@ -8599,7 +8646,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5">
       <c r="A198" t="s">
         <v>709</v>
       </c>
@@ -8616,7 +8663,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5">
       <c r="A199" t="s">
         <v>713</v>
       </c>
@@ -8633,7 +8680,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5">
       <c r="A200" t="s">
         <v>717</v>
       </c>
@@ -8650,7 +8697,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5">
       <c r="A201" t="s">
         <v>721</v>
       </c>
@@ -8667,7 +8714,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5">
       <c r="A202" t="s">
         <v>723</v>
       </c>
@@ -8684,7 +8731,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5">
       <c r="A203" t="s">
         <v>726</v>
       </c>
@@ -8701,7 +8748,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5">
       <c r="A204" t="s">
         <v>730</v>
       </c>
@@ -8718,7 +8765,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5">
       <c r="A205" t="s">
         <v>734</v>
       </c>
@@ -8735,7 +8782,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5">
       <c r="A206" t="s">
         <v>738</v>
       </c>
@@ -8752,7 +8799,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5">
       <c r="A207" t="s">
         <v>742</v>
       </c>
@@ -8769,7 +8816,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5">
       <c r="A208" t="s">
         <v>746</v>
       </c>
@@ -8786,7 +8833,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5">
       <c r="A209" t="s">
         <v>750</v>
       </c>
@@ -8803,7 +8850,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:5">
       <c r="A210" t="s">
         <v>754</v>
       </c>
@@ -8820,7 +8867,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:5">
       <c r="A211" t="s">
         <v>758</v>
       </c>
@@ -8837,7 +8884,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:5">
       <c r="A212" t="s">
         <v>762</v>
       </c>
@@ -8854,7 +8901,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:5">
       <c r="A213" t="s">
         <v>766</v>
       </c>
@@ -8871,7 +8918,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:5">
       <c r="A214" t="s">
         <v>770</v>
       </c>
@@ -8888,7 +8935,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:5">
       <c r="A215" t="s">
         <v>774</v>
       </c>
@@ -8905,7 +8952,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5">
       <c r="A216" t="s">
         <v>778</v>
       </c>
@@ -8922,7 +8969,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:5">
       <c r="A217" t="s">
         <v>781</v>
       </c>
@@ -8939,7 +8986,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5">
       <c r="A218" t="s">
         <v>785</v>
       </c>
@@ -8956,7 +9003,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5">
       <c r="A219" t="s">
         <v>789</v>
       </c>
@@ -8973,7 +9020,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5">
       <c r="A220" t="s">
         <v>793</v>
       </c>
@@ -8990,7 +9037,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5">
       <c r="A221" t="s">
         <v>797</v>
       </c>
@@ -9007,7 +9054,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5">
       <c r="A222" t="s">
         <v>800</v>
       </c>
@@ -9024,7 +9071,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:5">
       <c r="A223" t="s">
         <v>803</v>
       </c>
@@ -9041,7 +9088,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5">
       <c r="A224" t="s">
         <v>807</v>
       </c>
@@ -9058,7 +9105,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:5">
       <c r="A225" t="s">
         <v>811</v>
       </c>
@@ -9075,7 +9122,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:5">
       <c r="A226" t="s">
         <v>815</v>
       </c>
@@ -9092,7 +9139,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:5">
       <c r="A227" t="s">
         <v>819</v>
       </c>
@@ -9109,7 +9156,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:5">
       <c r="A228" t="s">
         <v>823</v>
       </c>
@@ -9126,7 +9173,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:5">
       <c r="A229" t="s">
         <v>827</v>
       </c>
@@ -9143,7 +9190,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:5">
       <c r="A230" t="s">
         <v>831</v>
       </c>
@@ -9160,7 +9207,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:5">
       <c r="A231" t="s">
         <v>835</v>
       </c>
@@ -9177,7 +9224,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:5">
       <c r="A232" t="s">
         <v>839</v>
       </c>
@@ -9194,7 +9241,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:5">
       <c r="A233" t="s">
         <v>843</v>
       </c>
@@ -9211,7 +9258,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:5">
       <c r="A234" t="s">
         <v>847</v>
       </c>
@@ -9228,7 +9275,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:5">
       <c r="A235" t="s">
         <v>851</v>
       </c>
@@ -9245,7 +9292,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:5">
       <c r="A236" t="s">
         <v>855</v>
       </c>
@@ -9262,7 +9309,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:5">
       <c r="A237" t="s">
         <v>859</v>
       </c>
@@ -9279,7 +9326,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:5">
       <c r="A238" t="s">
         <v>863</v>
       </c>
@@ -9296,7 +9343,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:5">
       <c r="A239" t="s">
         <v>867</v>
       </c>
@@ -9313,7 +9360,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:5">
       <c r="A240" t="s">
         <v>871</v>
       </c>
@@ -9330,7 +9377,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:5">
       <c r="A241" t="s">
         <v>875</v>
       </c>
@@ -9347,7 +9394,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:5">
       <c r="A242" t="s">
         <v>879</v>
       </c>
@@ -9364,7 +9411,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:5">
       <c r="A243" t="s">
         <v>883</v>
       </c>
@@ -9381,7 +9428,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:5">
       <c r="A244" t="s">
         <v>887</v>
       </c>
@@ -9398,7 +9445,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:5">
       <c r="A245" t="s">
         <v>891</v>
       </c>
@@ -9415,7 +9462,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:5">
       <c r="A246" t="s">
         <v>895</v>
       </c>
@@ -9432,7 +9479,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:5">
       <c r="A247" t="s">
         <v>899</v>
       </c>
@@ -9449,7 +9496,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:5">
       <c r="A248" t="s">
         <v>903</v>
       </c>
@@ -9466,7 +9513,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:5">
       <c r="A249" t="s">
         <v>907</v>
       </c>
@@ -9483,7 +9530,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:5">
       <c r="A250" t="s">
         <v>911</v>
       </c>
@@ -9500,7 +9547,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:5">
       <c r="A251" t="s">
         <v>915</v>
       </c>
@@ -9517,7 +9564,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:5">
       <c r="A252" t="s">
         <v>919</v>
       </c>
@@ -9534,7 +9581,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:5">
       <c r="A253" t="s">
         <v>923</v>
       </c>
@@ -9551,7 +9598,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:5">
       <c r="A254" t="s">
         <v>927</v>
       </c>
@@ -9568,7 +9615,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:5">
       <c r="A255" t="s">
         <v>930</v>
       </c>
@@ -9585,7 +9632,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:5">
       <c r="A256" t="s">
         <v>934</v>
       </c>
@@ -9602,7 +9649,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:5">
       <c r="A257" t="s">
         <v>935</v>
       </c>
@@ -9619,7 +9666,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:5">
       <c r="A258" t="s">
         <v>936</v>
       </c>
@@ -9636,7 +9683,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:5">
       <c r="A259" t="s">
         <v>940</v>
       </c>
@@ -9653,7 +9700,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:5">
       <c r="A260" t="s">
         <v>943</v>
       </c>
@@ -9670,7 +9717,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:5">
       <c r="A261" t="s">
         <v>944</v>
       </c>
@@ -9687,7 +9734,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:5">
       <c r="A262" t="s">
         <v>948</v>
       </c>
@@ -9704,7 +9751,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:5">
       <c r="A263" t="s">
         <v>951</v>
       </c>
@@ -9721,7 +9768,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:5">
       <c r="A264" t="s">
         <v>955</v>
       </c>
@@ -9738,7 +9785,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:5">
       <c r="A265" t="s">
         <v>959</v>
       </c>
@@ -9755,7 +9802,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:5">
       <c r="A266" t="s">
         <v>962</v>
       </c>
@@ -9772,7 +9819,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:5">
       <c r="A267" t="s">
         <v>966</v>
       </c>
@@ -9789,7 +9836,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:5">
       <c r="A268" t="s">
         <v>970</v>
       </c>
@@ -9806,7 +9853,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:5">
       <c r="A269" t="s">
         <v>971</v>
       </c>
@@ -9823,7 +9870,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:5">
       <c r="A270" t="s">
         <v>975</v>
       </c>
@@ -9840,7 +9887,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:5">
       <c r="A271" t="s">
         <v>979</v>
       </c>
@@ -9857,7 +9904,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:5">
       <c r="A272" t="s">
         <v>983</v>
       </c>
@@ -9874,7 +9921,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:5">
       <c r="A273" t="s">
         <v>987</v>
       </c>
@@ -9891,7 +9938,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:5">
       <c r="A274" t="s">
         <v>990</v>
       </c>
@@ -9908,7 +9955,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:5">
       <c r="A275" t="s">
         <v>994</v>
       </c>
@@ -9925,7 +9972,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:5">
       <c r="A276" t="s">
         <v>995</v>
       </c>
@@ -9942,7 +9989,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:5">
       <c r="A277" t="s">
         <v>999</v>
       </c>
@@ -9959,7 +10006,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:5">
       <c r="A278" t="s">
         <v>1003</v>
       </c>
@@ -9976,7 +10023,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:5">
       <c r="A279" t="s">
         <v>1007</v>
       </c>
@@ -9993,7 +10040,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:5">
       <c r="A280" t="s">
         <v>1011</v>
       </c>
@@ -10010,7 +10057,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:5">
       <c r="A281" t="s">
         <v>1015</v>
       </c>
@@ -10027,7 +10074,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:5">
       <c r="A282" t="s">
         <v>1018</v>
       </c>
@@ -10044,7 +10091,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:5">
       <c r="A283" t="s">
         <v>1020</v>
       </c>
@@ -10061,7 +10108,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:5">
       <c r="A284" t="s">
         <v>1023</v>
       </c>
@@ -10078,7 +10125,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:5">
       <c r="A285" t="s">
         <v>1027</v>
       </c>
@@ -10095,7 +10142,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:5">
       <c r="A286" t="s">
         <v>1031</v>
       </c>
@@ -10112,7 +10159,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:5">
       <c r="A287" t="s">
         <v>1035</v>
       </c>
@@ -10129,7 +10176,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:5">
       <c r="A288" t="s">
         <v>1039</v>
       </c>
@@ -10146,7 +10193,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:5">
       <c r="A289" t="s">
         <v>1043</v>
       </c>
@@ -10163,7 +10210,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:5">
       <c r="A290" t="s">
         <v>1047</v>
       </c>
@@ -10180,7 +10227,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:5">
       <c r="A291" t="s">
         <v>1051</v>
       </c>
@@ -10197,7 +10244,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:5">
       <c r="A292" t="s">
         <v>1054</v>
       </c>
@@ -10214,7 +10261,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:5">
       <c r="A293" t="s">
         <v>1055</v>
       </c>
@@ -10231,7 +10278,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:5">
       <c r="A294" t="s">
         <v>1059</v>
       </c>
@@ -10242,13 +10289,13 @@
         <v>1060</v>
       </c>
       <c r="D294" t="s">
-        <v>387</v>
+        <v>1623</v>
       </c>
       <c r="E294" t="s">
         <v>1061</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:5">
       <c r="A295" t="s">
         <v>1062</v>
       </c>
@@ -10265,7 +10312,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:5">
       <c r="A296" t="s">
         <v>1065</v>
       </c>
@@ -10282,7 +10329,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:5">
       <c r="A297" t="s">
         <v>1067</v>
       </c>
@@ -10299,7 +10346,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:5">
       <c r="A298" t="s">
         <v>1071</v>
       </c>
@@ -10316,7 +10363,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:5">
       <c r="A299" t="s">
         <v>1074</v>
       </c>
@@ -10333,7 +10380,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:5">
       <c r="A300" t="s">
         <v>1078</v>
       </c>
@@ -10350,7 +10397,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:5">
       <c r="A301" t="s">
         <v>1082</v>
       </c>
@@ -10367,7 +10414,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:5">
       <c r="A302" t="s">
         <v>1085</v>
       </c>
@@ -10384,7 +10431,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:5">
       <c r="A303" t="s">
         <v>1089</v>
       </c>
@@ -10401,7 +10448,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:5">
       <c r="A304" t="s">
         <v>1093</v>
       </c>
@@ -10418,7 +10465,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:5">
       <c r="A305" t="s">
         <v>1097</v>
       </c>
@@ -10435,7 +10482,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:5">
       <c r="A306" t="s">
         <v>1100</v>
       </c>
@@ -10452,7 +10499,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:5">
       <c r="A307" t="s">
         <v>1103</v>
       </c>
@@ -10469,7 +10516,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:5">
       <c r="A308" t="s">
         <v>1107</v>
       </c>
@@ -10486,7 +10533,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:5">
       <c r="A309" t="s">
         <v>1108</v>
       </c>
@@ -10503,7 +10550,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:5">
       <c r="A310" t="s">
         <v>1110</v>
       </c>
@@ -10520,7 +10567,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:5">
       <c r="A311" t="s">
         <v>1111</v>
       </c>
@@ -10537,7 +10584,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:5">
       <c r="A312" t="s">
         <v>1115</v>
       </c>
@@ -10554,7 +10601,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:5">
       <c r="A313" t="s">
         <v>1119</v>
       </c>
@@ -10571,7 +10618,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:5">
       <c r="A314" t="s">
         <v>1123</v>
       </c>
@@ -10588,7 +10635,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:5">
       <c r="A315" t="s">
         <v>1127</v>
       </c>
@@ -10605,7 +10652,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:5">
       <c r="A316" t="s">
         <v>1131</v>
       </c>
@@ -10622,7 +10669,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:5">
       <c r="A317" t="s">
         <v>1135</v>
       </c>
@@ -10639,7 +10686,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:5">
       <c r="A318" t="s">
         <v>1139</v>
       </c>
@@ -10656,7 +10703,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:5">
       <c r="A319" t="s">
         <v>1141</v>
       </c>
@@ -10673,7 +10720,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:5">
       <c r="A320" t="s">
         <v>1145</v>
       </c>
@@ -10690,7 +10737,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:5">
       <c r="A321" t="s">
         <v>1149</v>
       </c>
@@ -10707,7 +10754,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:5">
       <c r="A322" t="s">
         <v>1150</v>
       </c>
@@ -10724,7 +10771,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:5">
       <c r="A323" t="s">
         <v>1154</v>
       </c>
@@ -10741,7 +10788,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:5">
       <c r="A324" t="s">
         <v>1158</v>
       </c>
@@ -10758,7 +10805,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:5">
       <c r="A325" t="s">
         <v>1159</v>
       </c>
@@ -10775,7 +10822,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:5">
       <c r="A326" t="s">
         <v>1163</v>
       </c>
@@ -10792,7 +10839,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:5">
       <c r="A327" t="s">
         <v>1167</v>
       </c>
@@ -10809,7 +10856,7 @@
         <v>1169</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:5">
       <c r="A328" t="s">
         <v>1170</v>
       </c>
@@ -10826,7 +10873,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:5">
       <c r="A329" t="s">
         <v>1174</v>
       </c>
@@ -10843,7 +10890,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:5">
       <c r="A330" t="s">
         <v>1177</v>
       </c>
@@ -10860,7 +10907,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:5">
       <c r="A331" t="s">
         <v>1178</v>
       </c>
@@ -10877,7 +10924,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:5">
       <c r="A332" t="s">
         <v>1179</v>
       </c>
@@ -10894,7 +10941,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:5">
       <c r="A333" t="s">
         <v>1183</v>
       </c>
@@ -10911,7 +10958,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:5">
       <c r="A334" t="s">
         <v>1187</v>
       </c>
@@ -10928,7 +10975,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:5">
       <c r="A335" t="s">
         <v>1191</v>
       </c>
@@ -10945,7 +10992,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:5">
       <c r="A336" t="s">
         <v>1195</v>
       </c>
@@ -10962,7 +11009,7 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:5">
       <c r="A337" t="s">
         <v>1199</v>
       </c>
@@ -10979,7 +11026,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:5">
       <c r="A338" t="s">
         <v>1203</v>
       </c>
@@ -10996,7 +11043,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:5">
       <c r="A339" t="s">
         <v>1204</v>
       </c>
@@ -11013,7 +11060,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:5">
       <c r="A340" t="s">
         <v>1208</v>
       </c>
@@ -11030,7 +11077,7 @@
         <v>1211</v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:5">
       <c r="A341" t="s">
         <v>1212</v>
       </c>
@@ -11047,7 +11094,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:5">
       <c r="A342" t="s">
         <v>1213</v>
       </c>
@@ -11064,7 +11111,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:5">
       <c r="A343" t="s">
         <v>1216</v>
       </c>
@@ -11081,7 +11128,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:5">
       <c r="A344" t="s">
         <v>1220</v>
       </c>
@@ -11098,7 +11145,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:5">
       <c r="A345" t="s">
         <v>1224</v>
       </c>
@@ -11115,7 +11162,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:5">
       <c r="A346" t="s">
         <v>1228</v>
       </c>
@@ -11132,7 +11179,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:5">
       <c r="A347" t="s">
         <v>1229</v>
       </c>
@@ -11149,7 +11196,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:5">
       <c r="A348" t="s">
         <v>1233</v>
       </c>
@@ -11166,7 +11213,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:5">
       <c r="A349" t="s">
         <v>1237</v>
       </c>
@@ -11183,7 +11230,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:5">
       <c r="A350" t="s">
         <v>1238</v>
       </c>
@@ -11200,7 +11247,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:5">
       <c r="A351" t="s">
         <v>1240</v>
       </c>
@@ -11217,7 +11264,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:5">
       <c r="A352" t="s">
         <v>1244</v>
       </c>
@@ -11234,7 +11281,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:5">
       <c r="A353" t="s">
         <v>1248</v>
       </c>
@@ -11251,7 +11298,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:5">
       <c r="A354" t="s">
         <v>1249</v>
       </c>
@@ -11268,7 +11315,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:5">
       <c r="A355" t="s">
         <v>1253</v>
       </c>
@@ -11285,7 +11332,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:5">
       <c r="A356" t="s">
         <v>1257</v>
       </c>
@@ -11302,7 +11349,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:5">
       <c r="A357" t="s">
         <v>1260</v>
       </c>
@@ -11319,7 +11366,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:5">
       <c r="A358" t="s">
         <v>1264</v>
       </c>
@@ -11336,7 +11383,7 @@
         <v>1267</v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:5">
       <c r="A359" t="s">
         <v>1268</v>
       </c>
@@ -11353,7 +11400,7 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:5">
       <c r="A360" t="s">
         <v>1269</v>
       </c>
@@ -11370,7 +11417,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:5">
       <c r="A361" t="s">
         <v>1272</v>
       </c>
@@ -11387,7 +11434,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:5">
       <c r="A362" t="s">
         <v>1276</v>
       </c>
@@ -11404,7 +11451,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:5">
       <c r="A363" t="s">
         <v>1280</v>
       </c>
@@ -11421,7 +11468,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:5">
       <c r="A364" t="s">
         <v>1284</v>
       </c>
@@ -11438,7 +11485,7 @@
         <v>1287</v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:5">
       <c r="A365" t="s">
         <v>1288</v>
       </c>
@@ -11455,7 +11502,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:5">
       <c r="A366" t="s">
         <v>1291</v>
       </c>
@@ -11472,7 +11519,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:5">
       <c r="A367" t="s">
         <v>1295</v>
       </c>
@@ -11489,7 +11536,7 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:5">
       <c r="A368" t="s">
         <v>1299</v>
       </c>
@@ -11506,7 +11553,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:5">
       <c r="A369" t="s">
         <v>1303</v>
       </c>
@@ -11523,7 +11570,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:5">
       <c r="A370" t="s">
         <v>1307</v>
       </c>
@@ -11540,7 +11587,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:5">
       <c r="A371" t="s">
         <v>1311</v>
       </c>
@@ -11557,7 +11604,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:5">
       <c r="A372" t="s">
         <v>1315</v>
       </c>
@@ -11574,7 +11621,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:5">
       <c r="A373" t="s">
         <v>1319</v>
       </c>
@@ -11591,7 +11638,7 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:5">
       <c r="A374" t="s">
         <v>1320</v>
       </c>
@@ -11608,7 +11655,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:5">
       <c r="A375" t="s">
         <v>1324</v>
       </c>
@@ -11625,7 +11672,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:5">
       <c r="A376" t="s">
         <v>1327</v>
       </c>
@@ -11642,7 +11689,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:5">
       <c r="A377" t="s">
         <v>1331</v>
       </c>
@@ -11659,7 +11706,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:5">
       <c r="A378" t="s">
         <v>1334</v>
       </c>
@@ -11676,7 +11723,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:5">
       <c r="A379" t="s">
         <v>1336</v>
       </c>
@@ -11693,7 +11740,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:5">
       <c r="A380" t="s">
         <v>1340</v>
       </c>
@@ -11710,7 +11757,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="381" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:5">
       <c r="A381" t="s">
         <v>1344</v>
       </c>
@@ -11727,7 +11774,7 @@
         <v>1347</v>
       </c>
     </row>
-    <row r="382" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:5">
       <c r="A382" t="s">
         <v>1348</v>
       </c>
@@ -11744,7 +11791,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="383" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:5">
       <c r="A383" t="s">
         <v>1352</v>
       </c>
@@ -11761,7 +11808,7 @@
         <v>1355</v>
       </c>
     </row>
-    <row r="384" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:5">
       <c r="A384" t="s">
         <v>1356</v>
       </c>
@@ -11778,7 +11825,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="385" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:5">
       <c r="A385" t="s">
         <v>1360</v>
       </c>
@@ -11795,7 +11842,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="386" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:5">
       <c r="A386" t="s">
         <v>1364</v>
       </c>
@@ -11812,7 +11859,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="387" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:5">
       <c r="A387" t="s">
         <v>1366</v>
       </c>
@@ -11829,7 +11876,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="388" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:5">
       <c r="A388" t="s">
         <v>1370</v>
       </c>
@@ -11846,7 +11893,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="389" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:5">
       <c r="A389" t="s">
         <v>1374</v>
       </c>
@@ -11863,7 +11910,7 @@
         <v>1377</v>
       </c>
     </row>
-    <row r="390" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:5">
       <c r="A390" t="s">
         <v>1378</v>
       </c>
@@ -11880,7 +11927,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="391" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:5">
       <c r="A391" t="s">
         <v>1379</v>
       </c>
@@ -11897,7 +11944,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="392" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:5">
       <c r="A392" t="s">
         <v>1380</v>
       </c>
@@ -11914,7 +11961,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="393" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:5">
       <c r="A393" t="s">
         <v>1381</v>
       </c>
@@ -11931,7 +11978,7 @@
         <v>1384</v>
       </c>
     </row>
-    <row r="394" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:5">
       <c r="A394" t="s">
         <v>1385</v>
       </c>
@@ -11948,7 +11995,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="395" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:5">
       <c r="A395" t="s">
         <v>1389</v>
       </c>
@@ -11965,7 +12012,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="396" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:5">
       <c r="A396" t="s">
         <v>1393</v>
       </c>
@@ -11982,7 +12029,7 @@
         <v>1396</v>
       </c>
     </row>
-    <row r="397" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:5">
       <c r="A397" t="s">
         <v>1397</v>
       </c>
@@ -11999,7 +12046,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="398" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:5">
       <c r="A398" t="s">
         <v>1400</v>
       </c>
@@ -12016,7 +12063,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="399" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:5">
       <c r="A399" t="s">
         <v>1403</v>
       </c>
@@ -12033,7 +12080,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="400" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:5">
       <c r="A400" t="s">
         <v>1406</v>
       </c>
@@ -12050,7 +12097,7 @@
         <v>1407</v>
       </c>
     </row>
-    <row r="401" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:5">
       <c r="A401" t="s">
         <v>1408</v>
       </c>
@@ -12067,7 +12114,7 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="402" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:5">
       <c r="A402" t="s">
         <v>1412</v>
       </c>
@@ -12084,7 +12131,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="403" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:5">
       <c r="A403" t="s">
         <v>1416</v>
       </c>
@@ -12101,7 +12148,7 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="404" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:5">
       <c r="A404" t="s">
         <v>1420</v>
       </c>
@@ -12118,7 +12165,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="405" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:5">
       <c r="A405" t="s">
         <v>1424</v>
       </c>
@@ -12135,7 +12182,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="406" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:5">
       <c r="A406" t="s">
         <v>1428</v>
       </c>
@@ -12152,7 +12199,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="407" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:5">
       <c r="A407" t="s">
         <v>1431</v>
       </c>
@@ -12169,7 +12216,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="408" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:5">
       <c r="A408" t="s">
         <v>1435</v>
       </c>
@@ -12186,7 +12233,7 @@
         <v>1438</v>
       </c>
     </row>
-    <row r="409" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:5">
       <c r="A409" t="s">
         <v>1439</v>
       </c>
@@ -12203,7 +12250,7 @@
         <v>1443</v>
       </c>
     </row>
-    <row r="410" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:5">
       <c r="A410" t="s">
         <v>1444</v>
       </c>
@@ -12220,7 +12267,7 @@
         <v>1447</v>
       </c>
     </row>
-    <row r="411" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:5">
       <c r="A411" t="s">
         <v>1448</v>
       </c>
@@ -12237,7 +12284,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="412" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:5">
       <c r="A412" t="s">
         <v>1449</v>
       </c>
@@ -12254,7 +12301,7 @@
         <v>1452</v>
       </c>
     </row>
-    <row r="413" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:5">
       <c r="A413" t="s">
         <v>1453</v>
       </c>
@@ -12271,7 +12318,7 @@
         <v>1456</v>
       </c>
     </row>
-    <row r="414" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:5">
       <c r="A414" t="s">
         <v>1457</v>
       </c>
@@ -12288,7 +12335,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="415" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:5">
       <c r="A415" t="s">
         <v>1458</v>
       </c>
@@ -12305,7 +12352,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="416" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:5">
       <c r="A416" t="s">
         <v>1462</v>
       </c>
@@ -12322,7 +12369,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="417" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:5">
       <c r="A417" t="s">
         <v>1464</v>
       </c>
@@ -12339,7 +12386,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="418" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:5">
       <c r="A418" t="s">
         <v>1468</v>
       </c>
@@ -12356,7 +12403,7 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="419" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:5">
       <c r="A419" t="s">
         <v>1471</v>
       </c>
@@ -12373,7 +12420,7 @@
         <v>1474</v>
       </c>
     </row>
-    <row r="420" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:5">
       <c r="A420" t="s">
         <v>1475</v>
       </c>
@@ -12390,7 +12437,7 @@
         <v>1476</v>
       </c>
     </row>
-    <row r="421" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:5">
       <c r="A421" t="s">
         <v>1477</v>
       </c>
@@ -12407,7 +12454,7 @@
         <v>1480</v>
       </c>
     </row>
-    <row r="422" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:5">
       <c r="A422" t="s">
         <v>1481</v>
       </c>
@@ -12424,7 +12471,7 @@
         <v>1484</v>
       </c>
     </row>
-    <row r="423" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:5">
       <c r="A423" t="s">
         <v>1485</v>
       </c>
@@ -12441,7 +12488,7 @@
         <v>1488</v>
       </c>
     </row>
-    <row r="424" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:5">
       <c r="A424" t="s">
         <v>1489</v>
       </c>
@@ -12458,7 +12505,7 @@
         <v>1492</v>
       </c>
     </row>
-    <row r="425" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:5">
       <c r="A425" t="s">
         <v>1493</v>
       </c>
@@ -12475,7 +12522,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:5">
       <c r="A426" t="s">
         <v>1497</v>
       </c>
@@ -12492,7 +12539,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="427" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:5">
       <c r="A427" t="s">
         <v>1498</v>
       </c>
@@ -12509,7 +12556,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="428" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:5">
       <c r="A428" t="s">
         <v>1502</v>
       </c>
@@ -12526,7 +12573,7 @@
         <v>1505</v>
       </c>
     </row>
-    <row r="429" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:5">
       <c r="A429" t="s">
         <v>1506</v>
       </c>
@@ -12543,7 +12590,7 @@
         <v>1507</v>
       </c>
     </row>
-    <row r="430" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:5">
       <c r="A430" t="s">
         <v>1508</v>
       </c>
@@ -12560,7 +12607,7 @@
         <v>1511</v>
       </c>
     </row>
-    <row r="431" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:5">
       <c r="A431" t="s">
         <v>1512</v>
       </c>
@@ -12577,7 +12624,7 @@
         <v>1515</v>
       </c>
     </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:5">
       <c r="A432" t="s">
         <v>1516</v>
       </c>
@@ -12594,7 +12641,7 @@
         <v>1519</v>
       </c>
     </row>
-    <row r="433" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:5">
       <c r="A433" t="s">
         <v>1520</v>
       </c>
@@ -12611,7 +12658,7 @@
         <v>1523</v>
       </c>
     </row>
-    <row r="434" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:5">
       <c r="A434" t="s">
         <v>1524</v>
       </c>
@@ -12628,7 +12675,7 @@
         <v>1526</v>
       </c>
     </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:5">
       <c r="A435" t="s">
         <v>1527</v>
       </c>
@@ -12645,7 +12692,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="436" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:5">
       <c r="A436" t="s">
         <v>1528</v>
       </c>
@@ -12662,7 +12709,7 @@
         <v>1531</v>
       </c>
     </row>
-    <row r="437" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:5">
       <c r="A437" t="s">
         <v>1532</v>
       </c>
@@ -12679,7 +12726,7 @@
         <v>1535</v>
       </c>
     </row>
-    <row r="438" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:5">
       <c r="A438" t="s">
         <v>1536</v>
       </c>
@@ -12696,7 +12743,7 @@
         <v>1539</v>
       </c>
     </row>
-    <row r="439" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:5">
       <c r="A439" t="s">
         <v>1540</v>
       </c>
@@ -12713,7 +12760,7 @@
         <v>1542</v>
       </c>
     </row>
-    <row r="440" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:5">
       <c r="A440" t="s">
         <v>1543</v>
       </c>
@@ -12730,7 +12777,7 @@
         <v>1546</v>
       </c>
     </row>
-    <row r="441" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:5">
       <c r="A441" t="s">
         <v>1547</v>
       </c>
@@ -12747,7 +12794,7 @@
         <v>1550</v>
       </c>
     </row>
-    <row r="442" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:5">
       <c r="A442" t="s">
         <v>1551</v>
       </c>
@@ -12764,7 +12811,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="443" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:5">
       <c r="A443" t="s">
         <v>1555</v>
       </c>
@@ -12781,7 +12828,7 @@
         <v>1558</v>
       </c>
     </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:5">
       <c r="A444" t="s">
         <v>1559</v>
       </c>
@@ -12798,7 +12845,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:5">
       <c r="A445" t="s">
         <v>1563</v>
       </c>
@@ -12815,7 +12862,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="446" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:5">
       <c r="A446" t="s">
         <v>1564</v>
       </c>
@@ -12832,7 +12879,7 @@
         <v>1567</v>
       </c>
     </row>
-    <row r="447" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:5">
       <c r="A447" t="s">
         <v>1568</v>
       </c>
@@ -12849,7 +12896,7 @@
         <v>1571</v>
       </c>
     </row>
-    <row r="448" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:5">
       <c r="A448" t="s">
         <v>1572</v>
       </c>
@@ -12866,7 +12913,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="449" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:5">
       <c r="A449" t="s">
         <v>1574</v>
       </c>
@@ -12883,7 +12930,7 @@
         <v>1577</v>
       </c>
     </row>
-    <row r="450" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:5">
       <c r="A450" t="s">
         <v>1578</v>
       </c>
@@ -12900,7 +12947,7 @@
         <v>1581</v>
       </c>
     </row>
-    <row r="451" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:5">
       <c r="A451" t="s">
         <v>1582</v>
       </c>
@@ -12917,7 +12964,7 @@
         <v>1584</v>
       </c>
     </row>
-    <row r="452" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:5">
       <c r="A452" t="s">
         <v>1585</v>
       </c>
@@ -12934,7 +12981,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="453" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:5">
       <c r="A453" t="s">
         <v>1587</v>
       </c>
@@ -12951,7 +12998,7 @@
         <v>1590</v>
       </c>
     </row>
-    <row r="454" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:5">
       <c r="A454" t="s">
         <v>1591</v>
       </c>
@@ -12968,7 +13015,7 @@
         <v>1594</v>
       </c>
     </row>
-    <row r="455" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:5">
       <c r="A455" t="s">
         <v>1595</v>
       </c>
@@ -12985,7 +13032,7 @@
         <v>1598</v>
       </c>
     </row>
-    <row r="456" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:5">
       <c r="A456" t="s">
         <v>1599</v>
       </c>
@@ -13002,7 +13049,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="457" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:5">
       <c r="A457" t="s">
         <v>1600</v>
       </c>
@@ -13019,7 +13066,7 @@
         <v>1603</v>
       </c>
     </row>
-    <row r="458" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:5">
       <c r="A458" t="s">
         <v>1604</v>
       </c>
@@ -13036,7 +13083,7 @@
         <v>1607</v>
       </c>
     </row>
-    <row r="459" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:5">
       <c r="A459" t="s">
         <v>1608</v>
       </c>
@@ -13053,7 +13100,7 @@
         <v>1611</v>
       </c>
     </row>
-    <row r="460" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:5">
       <c r="A460" t="s">
         <v>1612</v>
       </c>
@@ -13070,7 +13117,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="461" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:5">
       <c r="A461" t="s">
         <v>1614</v>
       </c>
@@ -13090,5 +13137,11 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>